<commit_message>
changed orderbydesc on rides list
</commit_message>
<xml_diff>
--- a/MyRideTrackerWebApp-SeedData.xlsx
+++ b/MyRideTrackerWebApp-SeedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MyRideTrackerWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2804E6CD-20AE-49D0-BD61-AF412521DA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFFDC34-2511-4783-812E-079CB6784D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F49B623C-42DD-46D1-AB38-560E9CA613C6}"/>
   </bookViews>
@@ -30,6 +30,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>RideDate</t>
+  </si>
+  <si>
+    <t>MileageStart</t>
+  </si>
+  <si>
+    <t>MileageEnd</t>
+  </si>
+  <si>
+    <t>Fill Up</t>
+  </si>
+  <si>
+    <t>Gallons</t>
+  </si>
+  <si>
+    <t>PricePerGallon</t>
+  </si>
+  <si>
+    <t>RideRoute</t>
+  </si>
+  <si>
+    <t>RideDescription</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Gas Station</t>
+  </si>
+  <si>
+    <t>Initial Fill Up and Starting Ride</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Down to Nielsens, Lake Villa, IL</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +427,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA16180B-0197-45F1-BC25-CB1C3DB253FC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B2">
+        <v>415</v>
+      </c>
+      <c r="C2">
+        <v>415</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2">
+        <v>1.95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B3">
+        <v>415</v>
+      </c>
+      <c r="C3">
+        <v>485</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>